<commit_message>
add tax percantage in order import
</commit_message>
<xml_diff>
--- a/assets/sample_files/Order.xlsx
+++ b/assets/sample_files/Order.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\www\tiles\assets\sample_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB4632C-1D10-4C63-B41A-4CBBC85B3849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24B6DA02-7501-402A-AE29-1CD90CD133A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>location12</t>
   </si>
@@ -93,17 +87,20 @@
     <t>cn123</t>
   </si>
   <si>
-    <t>Unpai=0</t>
-  </si>
-  <si>
     <t>Paid=1</t>
+  </si>
+  <si>
+    <t>Tax %</t>
+  </si>
+  <si>
+    <t>Unpaid=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -299,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -493,21 +490,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3301C5B3-D879-4923-BE1F-F2EA1DB95DF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -519,7 +516,7 @@
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -556,8 +553,11 @@
       <c r="L1" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -594,8 +594,11 @@
       <c r="L2" s="1">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="N4" s="7" t="s">
         <v>16</v>
       </c>
@@ -603,33 +606,33 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="N7" s="5"/>
       <c r="O7" s="6"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{28C6F950-5626-485F-8C46-A04031FADB5D}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Add rate in impoert order,change samll to caps header in inocie and lpo pdf
</commit_message>
<xml_diff>
--- a/assets/sample_files/Order.xlsx
+++ b/assets/sample_files/Order.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>location12</t>
   </si>
@@ -36,12 +36,6 @@
     <t>sales_exp12.12</t>
   </si>
   <si>
-    <t>busylifeeasyway@yopmail.com</t>
-  </si>
-  <si>
-    <t>12,12</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>Unpaid=0</t>
+  </si>
+  <si>
+    <t>webtest1@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -490,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,72 +515,72 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
+        <v>382</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>120</v>
       </c>
       <c r="E2" s="1">
-        <v>12.12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>12.12</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
@@ -595,12 +592,12 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="N4" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -609,14 +606,14 @@
     <row r="5" spans="1:17">
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:17">
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P6" s="4"/>
     </row>

</xml_diff>